<commit_message>
Added All Gera and Raymie files. Waiting for their areas data. Updated the code
</commit_message>
<xml_diff>
--- a/CollectedData/RGData.xlsx
+++ b/CollectedData/RGData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2180" windowWidth="27360" windowHeight="15740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SampleE" sheetId="1" r:id="rId1"/>
+    <sheet name="SampleC" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>Load (lbs)</t>
   </si>
@@ -351,8 +352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F649"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5554,4 +5555,1235 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F152"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>23.47620392</v>
+      </c>
+      <c r="C2">
+        <v>-9.9170100000000004E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>57.031631470000001</v>
+      </c>
+      <c r="C3">
+        <v>-9.8778200000000007E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>74.866577149999998</v>
+      </c>
+      <c r="C4">
+        <v>-9.8771799999999993E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>88.260879520000003</v>
+      </c>
+      <c r="C5">
+        <v>-9.9190600000000004E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>100.76946259</v>
+      </c>
+      <c r="C6">
+        <v>-9.9028499999999995E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>114.92887878000001</v>
+      </c>
+      <c r="C7">
+        <v>-9.9123400000000004E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>130.67616272000001</v>
+      </c>
+      <c r="C8">
+        <v>-9.9195499999999992E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>145.64759827</v>
+      </c>
+      <c r="C9">
+        <v>-9.9096099999999993E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>159.24021912000001</v>
+      </c>
+      <c r="C10">
+        <v>-9.9189699999999992E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>169.22296143</v>
+      </c>
+      <c r="C11">
+        <v>-9.9285699999999994E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>175.42431640999999</v>
+      </c>
+      <c r="C12">
+        <v>-9.9280500000000008E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>181.5372467</v>
+      </c>
+      <c r="C13">
+        <v>-9.9294599999999993E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>185.83451843</v>
+      </c>
+      <c r="C14">
+        <v>-9.9398799999999999E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>188.32551574999999</v>
+      </c>
+      <c r="C15">
+        <v>-9.9491900000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>192.0841217</v>
+      </c>
+      <c r="C16">
+        <v>-9.9546300000000008E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>189.28225707999999</v>
+      </c>
+      <c r="C17">
+        <v>-9.9535999999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>201.26289367999999</v>
+      </c>
+      <c r="C18">
+        <v>-9.9548299999999996E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>207.14265442000001</v>
+      </c>
+      <c r="C19">
+        <v>-9.9443199999999995E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>212.92863464000001</v>
+      </c>
+      <c r="C20">
+        <v>-9.9425799999999995E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>217.203125</v>
+      </c>
+      <c r="C21">
+        <v>-9.9501799999999994E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>222.53752136</v>
+      </c>
+      <c r="C22">
+        <v>-9.9431599999999995E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>227.36944579999999</v>
+      </c>
+      <c r="C23">
+        <v>-9.9494900000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>232.33134459999999</v>
+      </c>
+      <c r="C24">
+        <v>-9.9377900000000002E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>239.08744812</v>
+      </c>
+      <c r="C25">
+        <v>-9.9400600000000006E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>246.00300598000001</v>
+      </c>
+      <c r="C26">
+        <v>-9.9420499999999992E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>250.3793335</v>
+      </c>
+      <c r="C27">
+        <v>-9.9391600000000007E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>256.68121337999997</v>
+      </c>
+      <c r="C28">
+        <v>-9.9402999999999991E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>263.94515990999997</v>
+      </c>
+      <c r="C29">
+        <v>-9.9365300000000007E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>268.96734619</v>
+      </c>
+      <c r="C30">
+        <v>-9.9390099999999999E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>275.70068358999998</v>
+      </c>
+      <c r="C31">
+        <v>-9.9485700000000003E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>282.61892699999999</v>
+      </c>
+      <c r="C32">
+        <v>-9.9339000000000007E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>289.45675659</v>
+      </c>
+      <c r="C33">
+        <v>-9.9213400000000007E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>296.7890625</v>
+      </c>
+      <c r="C34">
+        <v>-9.9292200000000008E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>303.63092040999999</v>
+      </c>
+      <c r="C35">
+        <v>-9.9277299999999992E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>308.91842651000002</v>
+      </c>
+      <c r="C36">
+        <v>-9.92934E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>316.85772704999999</v>
+      </c>
+      <c r="C37">
+        <v>-9.9249000000000004E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>323.92337035999998</v>
+      </c>
+      <c r="C38">
+        <v>-9.9352299999999998E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <v>331.40841675000001</v>
+      </c>
+      <c r="C39">
+        <v>-9.9166500000000008E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>339.66796875</v>
+      </c>
+      <c r="C40">
+        <v>-9.9059300000000003E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B41">
+        <v>347.61264038000002</v>
+      </c>
+      <c r="C41">
+        <v>-9.9119199999999994E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B42">
+        <v>347.86453246999997</v>
+      </c>
+      <c r="C42">
+        <v>-9.8958499999999994E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B43">
+        <v>361.15029907000002</v>
+      </c>
+      <c r="C43">
+        <v>-9.9177799999999993E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B44">
+        <v>370.18704223999998</v>
+      </c>
+      <c r="C44">
+        <v>-9.9045599999999998E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B45">
+        <v>376.99539184999998</v>
+      </c>
+      <c r="C45">
+        <v>-9.8956500000000006E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B46">
+        <v>385.37420653999999</v>
+      </c>
+      <c r="C46">
+        <v>-9.8835499999999996E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B47">
+        <v>394.09069823999999</v>
+      </c>
+      <c r="C47">
+        <v>-9.8868299999999992E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B48">
+        <v>399.45190430000002</v>
+      </c>
+      <c r="C48">
+        <v>-9.8797499999999996E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49">
+        <v>411.03588867000002</v>
+      </c>
+      <c r="C49">
+        <v>-9.8645399999999998E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B50">
+        <v>419.83544921999999</v>
+      </c>
+      <c r="C50">
+        <v>-9.8547200000000008E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>427.99987793000003</v>
+      </c>
+      <c r="C51">
+        <v>-9.8513999999999997E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B52">
+        <v>437.51495361000002</v>
+      </c>
+      <c r="C52">
+        <v>-9.84639E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B53">
+        <v>446.77011107999999</v>
+      </c>
+      <c r="C53">
+        <v>-9.8323200000000003E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B54">
+        <v>454.61026000999999</v>
+      </c>
+      <c r="C54">
+        <v>-9.8204E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B55">
+        <v>464.40136718999997</v>
+      </c>
+      <c r="C55">
+        <v>-9.8078100000000001E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B56">
+        <v>475.42929077000002</v>
+      </c>
+      <c r="C56">
+        <v>-9.8052599999999997E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B57">
+        <v>483.83892822000001</v>
+      </c>
+      <c r="C57">
+        <v>-9.7934600000000004E-3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B58">
+        <v>493.03109740999997</v>
+      </c>
+      <c r="C58">
+        <v>-9.7852800000000004E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B59">
+        <v>504.56149291999998</v>
+      </c>
+      <c r="C59">
+        <v>-9.7774100000000003E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B60">
+        <v>516.61315918000003</v>
+      </c>
+      <c r="C60">
+        <v>-9.7536900000000006E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B61">
+        <v>524.56317138999998</v>
+      </c>
+      <c r="C61">
+        <v>-9.7560600000000004E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B62">
+        <v>538.81103515999996</v>
+      </c>
+      <c r="C62">
+        <v>-9.7321300000000003E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B63">
+        <v>549.12072753999996</v>
+      </c>
+      <c r="C63">
+        <v>-9.7232199999999994E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B64">
+        <v>561.04510498000002</v>
+      </c>
+      <c r="C64">
+        <v>-9.7034700000000005E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B65">
+        <v>574.47827147999999</v>
+      </c>
+      <c r="C65">
+        <v>-9.7084200000000006E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B66">
+        <v>585.48339843999997</v>
+      </c>
+      <c r="C66">
+        <v>-9.6833700000000002E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B67">
+        <v>596.95886229999996</v>
+      </c>
+      <c r="C67">
+        <v>-9.6623899999999999E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B68">
+        <v>607.44409180000002</v>
+      </c>
+      <c r="C68">
+        <v>-9.6611200000000005E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B69">
+        <v>616.78631591999999</v>
+      </c>
+      <c r="C69">
+        <v>-9.6471899999999999E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B70">
+        <v>631.67736816000001</v>
+      </c>
+      <c r="C70">
+        <v>-9.6231700000000003E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B71">
+        <v>645.97210693</v>
+      </c>
+      <c r="C71">
+        <v>-9.6133099999999999E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B72">
+        <v>656.61413574000005</v>
+      </c>
+      <c r="C72">
+        <v>-9.6066399999999996E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B73">
+        <v>662.92535399999997</v>
+      </c>
+      <c r="C73">
+        <v>-9.5924300000000007E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B74">
+        <v>680.16003418000003</v>
+      </c>
+      <c r="C74">
+        <v>-9.5832899999999995E-3</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B75">
+        <v>694.89831543000003</v>
+      </c>
+      <c r="C75">
+        <v>-9.5769800000000006E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B76">
+        <v>696.90826416000004</v>
+      </c>
+      <c r="C76">
+        <v>-9.5553200000000008E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B77">
+        <v>715.09429932</v>
+      </c>
+      <c r="C77">
+        <v>-9.5384900000000002E-3</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B78">
+        <v>732.01940918000003</v>
+      </c>
+      <c r="C78">
+        <v>-9.5332899999999998E-3</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B79">
+        <v>747.74658203000001</v>
+      </c>
+      <c r="C79">
+        <v>-9.5160499999999999E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B80">
+        <v>760.10638428000004</v>
+      </c>
+      <c r="C80">
+        <v>-9.4943000000000007E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B81">
+        <v>766.83972168000003</v>
+      </c>
+      <c r="C81">
+        <v>-9.4768400000000003E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B82">
+        <v>786.01867675999995</v>
+      </c>
+      <c r="C82">
+        <v>-9.4696299999999997E-3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B83">
+        <v>792.85919189000003</v>
+      </c>
+      <c r="C83">
+        <v>-9.4491499999999999E-3</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B84">
+        <v>806.66351318</v>
+      </c>
+      <c r="C84">
+        <v>-9.43103E-3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B85">
+        <v>823.38092041000004</v>
+      </c>
+      <c r="C85">
+        <v>-9.4101099999999993E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B86">
+        <v>840.16802978999999</v>
+      </c>
+      <c r="C86">
+        <v>-9.3958700000000006E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B87">
+        <v>850.84356689000003</v>
+      </c>
+      <c r="C87">
+        <v>-9.3719100000000007E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B88">
+        <v>867.54620361000002</v>
+      </c>
+      <c r="C88">
+        <v>-9.3633199999999996E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B89">
+        <v>882.19207763999998</v>
+      </c>
+      <c r="C89">
+        <v>-9.3469899999999995E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B90">
+        <v>895.41485595999995</v>
+      </c>
+      <c r="C90">
+        <v>-9.3191699999999999E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B91">
+        <v>909.71362305000002</v>
+      </c>
+      <c r="C91">
+        <v>-9.2921099999999993E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B92">
+        <v>920.2578125</v>
+      </c>
+      <c r="C92">
+        <v>-9.2909900000000007E-3</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B93">
+        <v>936.79028319999998</v>
+      </c>
+      <c r="C93">
+        <v>-9.2682700000000003E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B94">
+        <v>955.41046143000005</v>
+      </c>
+      <c r="C94">
+        <v>-9.2485999999999992E-3</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B95">
+        <v>971.19793701000003</v>
+      </c>
+      <c r="C95">
+        <v>-9.2207799999999996E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B96">
+        <v>985.92950439000003</v>
+      </c>
+      <c r="C96">
+        <v>-9.2032699999999995E-3</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B97">
+        <v>1000.20019531</v>
+      </c>
+      <c r="C97">
+        <v>-9.1786100000000002E-3</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B98">
+        <v>1015.3283691399999</v>
+      </c>
+      <c r="C98">
+        <v>-9.1548700000000007E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B99">
+        <v>1024.7336425799999</v>
+      </c>
+      <c r="C99">
+        <v>-9.1550399999999997E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B100">
+        <v>1042.84729004</v>
+      </c>
+      <c r="C100">
+        <v>-9.1199000000000002E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B101">
+        <v>1062.6264648399999</v>
+      </c>
+      <c r="C101">
+        <v>-9.0856099999999992E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B102">
+        <v>1077.88464355</v>
+      </c>
+      <c r="C102">
+        <v>-9.0645699999999992E-3</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B103">
+        <v>1093.94824219</v>
+      </c>
+      <c r="C103">
+        <v>-9.04399E-3</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B104">
+        <v>1110.6817627</v>
+      </c>
+      <c r="C104">
+        <v>-9.0147100000000004E-3</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B105">
+        <v>1120.00390625</v>
+      </c>
+      <c r="C105">
+        <v>-8.9944900000000008E-3</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B106">
+        <v>1137.97949219</v>
+      </c>
+      <c r="C106">
+        <v>-8.9818099999999998E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B107">
+        <v>1157.5792236299999</v>
+      </c>
+      <c r="C107">
+        <v>-8.9398800000000007E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B108">
+        <v>1173.2634277300001</v>
+      </c>
+      <c r="C108">
+        <v>-8.9164699999999993E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B109">
+        <v>1191.4561767600001</v>
+      </c>
+      <c r="C109">
+        <v>-8.8892599999999995E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B110">
+        <v>1208.5715332</v>
+      </c>
+      <c r="C110">
+        <v>-8.8441700000000002E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B111">
+        <v>1219.07421875</v>
+      </c>
+      <c r="C111">
+        <v>-8.8254200000000005E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B112">
+        <v>1237.21606445</v>
+      </c>
+      <c r="C112">
+        <v>-8.8028299999999993E-3</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B113">
+        <v>1256.7755127</v>
+      </c>
+      <c r="C113">
+        <v>-8.78111E-3</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B114">
+        <v>1272.2561035199999</v>
+      </c>
+      <c r="C114">
+        <v>-8.7338499999999996E-3</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B115">
+        <v>1289.4787597699999</v>
+      </c>
+      <c r="C115">
+        <v>-8.7016699999999999E-3</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B116">
+        <v>1308.0935058600001</v>
+      </c>
+      <c r="C116">
+        <v>-8.6794899999999998E-3</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B117">
+        <v>1320.72265625</v>
+      </c>
+      <c r="C117">
+        <v>-8.6396200000000006E-3</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B118">
+        <v>1338.85778809</v>
+      </c>
+      <c r="C118">
+        <v>-8.6234799999999993E-3</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B119">
+        <v>1359.4919433600001</v>
+      </c>
+      <c r="C119">
+        <v>-8.5760400000000001E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B120">
+        <v>1376.5122070299999</v>
+      </c>
+      <c r="C120">
+        <v>-8.5233199999999992E-3</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B121">
+        <v>1391.1593017600001</v>
+      </c>
+      <c r="C121">
+        <v>-8.5018100000000003E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B122">
+        <v>1407.7401123</v>
+      </c>
+      <c r="C122">
+        <v>-8.4735000000000001E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B123">
+        <v>1426.3615722699999</v>
+      </c>
+      <c r="C123">
+        <v>-8.4462900000000004E-3</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B124">
+        <v>1445.8192138700001</v>
+      </c>
+      <c r="C124">
+        <v>-8.3751499999999996E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B125">
+        <v>1461.0975341799999</v>
+      </c>
+      <c r="C125">
+        <v>-8.35289E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B126">
+        <v>1477.4250488299999</v>
+      </c>
+      <c r="C126">
+        <v>-8.3084000000000005E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B127">
+        <v>1497.60217285</v>
+      </c>
+      <c r="C127">
+        <v>-8.2827700000000001E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B128">
+        <v>1515.0954589800001</v>
+      </c>
+      <c r="C128">
+        <v>-8.2246400000000001E-3</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B129">
+        <v>1527.78356934</v>
+      </c>
+      <c r="C129">
+        <v>-8.2101799999999992E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B130">
+        <v>1545.109375</v>
+      </c>
+      <c r="C130">
+        <v>-8.1446599999999997E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B131">
+        <v>1565.9110107399999</v>
+      </c>
+      <c r="C131">
+        <v>-8.1189899999999995E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B132">
+        <v>1583.3962402300001</v>
+      </c>
+      <c r="C132">
+        <v>-8.0811800000000003E-3</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B133">
+        <v>1597.2380371100001</v>
+      </c>
+      <c r="C133">
+        <v>-8.0206500000000007E-3</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B134">
+        <v>1615.40002441</v>
+      </c>
+      <c r="C134">
+        <v>-7.9745800000000002E-3</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B135">
+        <v>1634.3391113299999</v>
+      </c>
+      <c r="C135">
+        <v>-7.9182100000000002E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B136">
+        <v>1652.0292968700001</v>
+      </c>
+      <c r="C136">
+        <v>-7.8810900000000003E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B137">
+        <v>1664.1640625</v>
+      </c>
+      <c r="C137">
+        <v>-7.8363300000000007E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B138">
+        <v>1682.0069580100001</v>
+      </c>
+      <c r="C138">
+        <v>-7.7956800000000001E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B139">
+        <v>1703.30310059</v>
+      </c>
+      <c r="C139">
+        <v>-7.7305100000000003E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B140">
+        <v>1721.9835205100001</v>
+      </c>
+      <c r="C140">
+        <v>-7.6703099999999996E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B141">
+        <v>1730.5700683600001</v>
+      </c>
+      <c r="C141">
+        <v>-7.6335200000000004E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B142">
+        <v>1751.2739257799999</v>
+      </c>
+      <c r="C142">
+        <v>-7.5642299999999999E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B143">
+        <v>1770.7932128899999</v>
+      </c>
+      <c r="C143">
+        <v>-7.5193500000000002E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B144">
+        <v>1787.2104492200001</v>
+      </c>
+      <c r="C144">
+        <v>-7.4507100000000001E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B145">
+        <v>1793.24157715</v>
+      </c>
+      <c r="C145">
+        <v>-7.4015599999999997E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B146">
+        <v>1820.8060302700001</v>
+      </c>
+      <c r="C146">
+        <v>-7.34061E-3</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B147">
+        <v>1836.38049316</v>
+      </c>
+      <c r="C147">
+        <v>-7.2600199999999998E-3</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B148">
+        <v>1854.4499511700001</v>
+      </c>
+      <c r="C148">
+        <v>-7.1993300000000003E-3</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B149">
+        <v>1871.9458007799999</v>
+      </c>
+      <c r="C149">
+        <v>-7.1363399999999997E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B150">
+        <v>1879.42150879</v>
+      </c>
+      <c r="C150">
+        <v>-7.08488E-3</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B151">
+        <v>-1.2957466799999999</v>
+      </c>
+      <c r="C151">
+        <v>6.0262E-4</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B152">
+        <v>-0.83479833999999997</v>
+      </c>
+      <c r="C152">
+        <v>6.0815999999999995E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>